<commit_message>
Finished Vampire skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/2_Hunter/Documentation/HunterSkills.xlsx
+++ b/GameDesign/Class/_Done/2_Hunter/Documentation/HunterSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="1-DistortionArea" sheetId="1" r:id="rId1"/>
@@ -2062,7 +2062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -2414,8 +2414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Worked on the stats and effect doc. + Cleaned Hunter skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/2_Hunter/Documentation/HunterSkills.xlsx
+++ b/GameDesign/Class/_Done/2_Hunter/Documentation/HunterSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-DistortionArea" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
   <si>
     <t>Additional Info</t>
   </si>
@@ -86,18 +86,12 @@
     <t>On target: [[Area of effect: - Single cell]]</t>
   </si>
   <si>
-    <t>Push 2 cells in the opposite direction of the spell cast point.</t>
-  </si>
-  <si>
     <t>Glowing Arrow</t>
   </si>
   <si>
     <t>[[AP: 3 ]]</t>
   </si>
   <si>
-    <t>[[Max effect accumulation: 00 ]]</t>
-  </si>
-  <si>
     <t>On Distortion Area: [[Area of effect: - 8 Singles cells]]</t>
   </si>
   <si>
@@ -149,33 +143,12 @@
     <t>[[Range: 2-3 ]]</t>
   </si>
   <si>
-    <t>[[Max effect accumulation: 1 ]]</t>
-  </si>
-  <si>
     <t>[[Area of effect: - Single cell ]]</t>
   </si>
   <si>
-    <t>Effect name: ''Blood Mark''.</t>
-  </si>
-  <si>
-    <t>Self: If not under ''Blood Mark'' effect, [[Blood Mark]] (00 turns)</t>
-  </si>
-  <si>
-    <t>Self: If not under ''Blood Mark'' effect, -30% HP from max hp</t>
-  </si>
-  <si>
-    <t>If not under ''Blood Mark'' effect: [[Damage: 75 fire ]]</t>
-  </si>
-  <si>
-    <t>If under ''Blood Mark'' effect: [[Damage: 75 fire + 75 dark ]]</t>
-  </si>
-  <si>
     <t>Poison Arrow</t>
   </si>
   <si>
-    <t>[[Max effect accumulation: 3 ]]</t>
-  </si>
-  <si>
     <t>[[Number of casts per turn: 2 ]]</t>
   </si>
   <si>
@@ -185,15 +158,6 @@
     <t>[[Range: 1-5 ]]</t>
   </si>
   <si>
-    <t>If not under ''Blood Mark'' effect: [[Damage:  25 dark ]] (2 turns)</t>
-  </si>
-  <si>
-    <t>If under ''Blood Mark'' effect: [[Damage:  25 dark ]] (3 turns)</t>
-  </si>
-  <si>
-    <t>Effect name: ''Poison''.</t>
-  </si>
-  <si>
     <t>Survival</t>
   </si>
   <si>
@@ -206,15 +170,6 @@
     <t>[[Number of turns between two casts: 5 ]]</t>
   </si>
   <si>
-    <t>[[Boost MP by current iteself]] (1 turn)</t>
-  </si>
-  <si>
-    <t>[[Boost HP by 15% of max HP]] (3 turns)</t>
-  </si>
-  <si>
-    <t>Effect name: ''Survival''.</t>
-  </si>
-  <si>
     <t>Canis Lupus</t>
   </si>
   <si>
@@ -227,30 +182,15 @@
     <t>[[Number of turns between two casts: 8 ]]</t>
   </si>
   <si>
-    <t>Summon a ''Canis Lupus'' [[25% of hunter max HP, 5 AP, 5 MP, 30% earth resistence, -10% fire resistence, -30% water resistence, 10% air resistence, -30% light resistence, 30% dark resistence]]</t>
-  </si>
-  <si>
     <t>Infected Bite</t>
   </si>
   <si>
     <t>[[Range: 1 ]]</t>
   </si>
   <si>
-    <t>[[Max effect accumulation: 2 ]]</t>
-  </si>
-  <si>
     <t>Last Resort</t>
   </si>
   <si>
-    <t>Effect name: ''Treason''.</t>
-  </si>
-  <si>
-    <t>Self: [[Treason effect ]] (00 turns)</t>
-  </si>
-  <si>
-    <t>Target: Unsummon ''Canis Lupus''.</t>
-  </si>
-  <si>
     <t>[[Number of turns between two casts: 00 ]]</t>
   </si>
   <si>
@@ -260,65 +200,338 @@
     <t>On Distortion Area: [[Area of effect: - 3 Singles cells]]</t>
   </si>
   <si>
-    <t>[[Damage:  (50 - (10 * obstacle crossed)) earth ]]</t>
-  </si>
-  <si>
-    <t>[[Damage: 5-10 earth ]]                                                      [[Damage: 20 dark ]] (2 turns)</t>
-  </si>
-  <si>
-    <t>Inflicts Earth-type damage and give poisons that inflicts Dark-type damage.</t>
-  </si>
-  <si>
     <t>Summons a Distortion Area that dosn't block the field of view.  Affect other skills of the caster.</t>
   </si>
   <si>
-    <t>[[Damage:  25-30 air ]]</t>
-  </si>
-  <si>
-    <t>Inflicts Air-type damage on enemies.                                             Push the target.                                                                              When targeting the Distortion Area, the skill is replicated on each straight line of the Distortion Area exept the line of the caster.     The first obstacle encountered stop the skill progression.</t>
-  </si>
-  <si>
     <t>Inflicts Light-type damage on enemies.                                        Reduce range of enemies.                                                                                 When targeting the Distortion Area, the skill is replicated on each straight and diagonal line of the Distortion Area and heal caster and allies when touching them.                                                               The first obstacle encountered stop the skill progression.</t>
   </si>
   <si>
-    <t>[[Damage:  15-20 light ]]</t>
-  </si>
-  <si>
-    <t>[[Reduce range by 1]] (2 turns)</t>
-  </si>
-  <si>
-    <t>From Distortion Area: [[Heal:  15-20 light ]]</t>
-  </si>
-  <si>
-    <t>Inflicts Light-type damage.                                                         Infinite range and cross every obstacle, but the damage decrease for each obstacle crossed.</t>
-  </si>
-  <si>
     <t>Inflicts Light-type damage on impact and Fire-type damage on the burning area.                                                                                     The burning area dealt damage for every burning cell crossed.</t>
   </si>
   <si>
-    <t>Inflicts Fire-type damage if the caster isn't under Blood Mark effect, otherwise inflicts Fire-type and Dark-type damage.                                             If the caster isn't under Blood Mark effect, reduce caster HP and give the effect, otherwise only remove the effect.</t>
-  </si>
-  <si>
-    <t>Poisons that inflicts Dark-type damage.                                           The poison last longer if the caster is under Blood Mark effect.</t>
-  </si>
-  <si>
     <t>Increases the caster HP and MP temporarily.                                  Can only be used when the caster has 25% or less HP remaning.</t>
   </si>
   <si>
-    <t>Summons a Canis Lupus which poison the enemies.                      Can only be used if the caster is not under the Treason effect.</t>
-  </si>
-  <si>
     <t>Heal the caster but unsummon the Canis Lupus and preven from summoning it for the rest of the fight.                                              Can only be used when targeting the caster Canis Lupus.</t>
   </si>
   <si>
-    <t>Self: [[Heal: The max HP of ''Canis Lupus'' ]]</t>
+    <t>Inflicts Wind-type damage on enemies.                                             Push the target.                                                                              When targeting the Distortion Area, the skill is replicated on each straight line of the Distortion Area exept the line of the caster.     The first obstacle encountered stop the skill progression.</t>
+  </si>
+  <si>
+    <t>[[Damage:  25-30 wind ]]</t>
+  </si>
+  <si>
+    <t>Push 2 cells in the opposite direction of the caster.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage:  15-20 light ]]</t>
+  </si>
+  <si>
+    <t>If direct hit:</t>
+  </si>
+  <si>
+    <t>If hit from ''Distortion Area'':</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Caster and allies: [[Heal:  15-20 light ]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Ennemies: [[Damage:  15-20 light ]]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    [[Blindness]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +2 level (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Ennemies: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Blindness]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +1 level (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>Inflicts Ground-type damage.                                                         Infinite range and cross every obstacle, but the damage decrease for each obstacle crossed.</t>
+  </si>
+  <si>
+    <t>[[Damage:  (50 - (10 * obstacle crossed)) ground ]]</t>
+  </si>
+  <si>
+    <t>Inflicts Fire-type damage if the caster dosn't have Blood Mark effect, otherwise inflicts Fire-type and Dark-type damage.                                             If the caster dosn't have Blood Mark effect, reduce caster HP and give the effect, otherwise only remove the effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage: 75 fire + 75 dark ]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If caster have </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Blood Mark]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If caster doesn’t have </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Blood Mark]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage: 75 fire ]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Self: [[Damage: 30% Max HP ]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Self: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Blood Mark]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Self: Remove </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Blood Mark]]</t>
+    </r>
+  </si>
+  <si>
+    <t>Poisons that inflicts Dark-type damage.                                           The poison last longer if the caster have Blood Mark effect.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    [[Poison]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +25 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    [[Poison]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +25 levels (3 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Vitality]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +15 levels (3 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Speed]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +(Current MP) levels (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>Summon a ''Canis Lupus'' [[25% of caster Max HP, 5 AP, 5 MP, 30% ground resistence, -10% fire resistence, -30% water resistence, 10% wind resistence, -30% light resistence, 30% dark resistence]]</t>
+  </si>
+  <si>
+    <t>Summons a Canis Lupus which poison the enemies.                      Can only be used if the caster is not under the Loneliness effect.</t>
+  </si>
+  <si>
+    <t>Inflicts Ground-type damage and give poisons that inflicts Dark-type damage.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[[Damage: 5-10 ground ]]                                                      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[[Poison]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>+20 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>Self: [[Heal: 25% HP ]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Self: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Loneliness]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>Unsummon ''Canis Lupus''.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +571,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -391,7 +610,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -441,17 +660,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -485,7 +693,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -503,8 +711,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,7 +1062,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -980,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D27"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1211,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1015,7 +1223,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1034,14 +1242,14 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1053,7 +1261,7 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -1065,89 +1273,80 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
-        <v>92</v>
+      <c r="C18" s="16" t="s">
+        <v>89</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="2" t="s">
-        <v>70</v>
+      <c r="C19" s="17" t="s">
+        <v>90</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="5"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1160,7 +1359,7 @@
   <dimension ref="B2:D27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1391,7 @@
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="15" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1268,7 +1467,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1280,14 +1479,14 @@
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="18" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="18" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1332,10 +1531,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D30"/>
+  <dimension ref="B2:D32"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,7 +1554,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1367,7 +1566,7 @@
     <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1379,14 +1578,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1423,8 +1622,8 @@
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="6" t="s">
-        <v>20</v>
+      <c r="C14" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1436,87 +1635,103 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="2" t="s">
-        <v>21</v>
+      <c r="C19" s="19" t="s">
+        <v>64</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="19" t="s">
+        <v>63</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="18" t="s">
-        <v>82</v>
+      <c r="C21" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="18" t="s">
-        <v>83</v>
+      <c r="C22" s="19" t="s">
+        <v>65</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="18" t="s">
-        <v>84</v>
+      <c r="C23" s="19" t="s">
+        <v>66</v>
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="19" t="s">
+        <v>67</v>
+      </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B25" s="1"/>
+      <c r="C25" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B27" s="1"/>
-      <c r="C27" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1"/>
-    </row>
+    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B29" s="1"/>
-      <c r="C29" s="9"/>
+      <c r="C29" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="5"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B31" s="1"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1529,7 +1744,7 @@
   <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,7 +1764,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1561,7 +1776,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1580,7 +1795,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1592,7 +1807,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -1630,7 +1845,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1642,7 +1857,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1710,7 +1925,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1722,7 +1937,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1741,7 +1956,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1779,7 +1994,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1791,14 +2006,14 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1810,21 +2025,21 @@
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1869,10 +2084,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D29"/>
+  <dimension ref="B2:D31"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,7 +2107,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1904,7 +2119,7 @@
     <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1916,14 +2131,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1967,90 +2182,102 @@
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="C18" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="16" t="s">
-        <v>43</v>
+      <c r="C19" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="19" t="s">
-        <v>42</v>
+      <c r="C20" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="17" t="s">
-        <v>41</v>
+      <c r="C21" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B24" s="1"/>
+      <c r="C24" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B26" s="1"/>
-      <c r="C26" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="1"/>
-    </row>
+    <row r="26" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B28" s="1"/>
-      <c r="C28" s="8" t="s">
-        <v>40</v>
+      <c r="C28" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="5"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B30" s="1"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2063,7 +2290,7 @@
   <dimension ref="B2:D29"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,7 +2310,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2095,7 +2322,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2107,14 +2334,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2151,58 +2378,60 @@
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="6" t="s">
-        <v>46</v>
+      <c r="C14" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2231,9 +2460,7 @@
     </row>
     <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
-      <c r="C28" s="8" t="s">
-        <v>52</v>
-      </c>
+      <c r="C28" s="8"/>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -2249,10 +2476,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D25"/>
+  <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2272,7 +2499,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2284,7 +2511,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="15" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2296,14 +2523,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2315,7 +2542,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -2327,82 +2554,73 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="C16" s="16" t="s">
+        <v>83</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>58</v>
+      <c r="C17" s="17" t="s">
+        <v>84</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="5"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2414,8 +2632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H26" sqref="F1:H26"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2432,7 +2650,7 @@
     <row r="1" spans="2:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
       <c r="G1" s="10" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2447,12 +2665,12 @@
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="7" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2467,12 +2685,12 @@
     <row r="5" spans="2:8" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="14" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2487,19 +2705,19 @@
     <row r="7" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
@@ -2509,12 +2727,12 @@
     <row r="9" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="2" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -2529,12 +2747,12 @@
     <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -2555,9 +2773,7 @@
       </c>
       <c r="D13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="6" t="s">
-        <v>67</v>
-      </c>
+      <c r="G13" s="6"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
@@ -2571,7 +2787,7 @@
     <row r="15" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
@@ -2609,12 +2825,12 @@
     <row r="19" spans="2:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="11" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="12" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="H19" s="1"/>
     </row>

</xml_diff>

<commit_message>
Worked on the Effects doc. + Cleaned the Elementalist skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/2_Hunter/Documentation/HunterSkills.xlsx
+++ b/GameDesign/Class/_Done/2_Hunter/Documentation/HunterSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1-DistortionArea" sheetId="1" r:id="rId1"/>
@@ -125,13 +125,7 @@
     <t>Impact: [[Area of effect: - Single cell ]]</t>
   </si>
   <si>
-    <t>Burning Ground: [[Damage:  25 fire ]]</t>
-  </si>
-  <si>
     <t>Impact: [[Damage:  20-30 light ]]</t>
-  </si>
-  <si>
-    <t>Burning Ground (3 turns)</t>
   </si>
   <si>
     <t>Cursed Arrow</t>
@@ -525,6 +519,12 @@
   </si>
   <si>
     <t>Unsummon ''Canis Lupus''.</t>
+  </si>
+  <si>
+    <t>'Burning Ground'' (Active Glyph) (3 turns):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage: 25 fire ]]</t>
   </si>
 </sst>
 </file>
@@ -672,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -713,6 +713,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1062,7 +1064,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1190,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1213,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1223,7 +1225,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1242,14 +1244,14 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1273,7 +1275,7 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1297,21 +1299,21 @@
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1391,7 +1393,7 @@
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1467,7 +1469,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1479,14 +1481,14 @@
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -1566,7 +1568,7 @@
     <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1654,49 +1656,49 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
       <c r="C25" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1776,7 +1778,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1857,7 +1859,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1937,7 +1939,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2025,21 +2027,21 @@
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="16" t="s">
-        <v>32</v>
+      <c r="C20" s="21" t="s">
+        <v>90</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="17" t="s">
-        <v>30</v>
+      <c r="C21" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -2086,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D31"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,7 +2109,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2119,7 +2121,7 @@
     <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2131,14 +2133,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2188,7 +2190,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -2200,49 +2202,49 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -2310,7 +2312,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2322,7 +2324,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2341,7 +2343,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2379,14 +2381,14 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2410,28 +2412,28 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2499,7 +2501,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2511,7 +2513,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2523,14 +2525,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2554,7 +2556,7 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2578,14 +2580,14 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2650,7 +2652,7 @@
     <row r="1" spans="2:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
       <c r="G1" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2665,12 +2667,12 @@
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2685,12 +2687,12 @@
     <row r="5" spans="2:8" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2705,7 +2707,7 @@
     <row r="7" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="1"/>
@@ -2717,7 +2719,7 @@
     <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
@@ -2727,12 +2729,12 @@
     <row r="9" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -2787,7 +2789,7 @@
     <row r="15" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
@@ -2825,12 +2827,12 @@
     <row r="19" spans="2:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H19" s="1"/>
     </row>

</xml_diff>

<commit_message>
- Hunter and Ninja skill simplified.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/2_Hunter/Documentation/HunterSkills.xlsx
+++ b/GameDesign/Class/_Done/2_Hunter/Documentation/HunterSkills.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Client\Desktop\My_Dev\BattleForVoxturia\GameDesign\Class\_Done\2_Hunter\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sébastien Godbout\Desktop\_MyDev\BattleForVoxturia\GameDesign\Class\_Done\2_Hunter\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-DistortionArea" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="9-CanisLupus" sheetId="9" r:id="rId9"/>
     <sheet name="10-LastResort" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="91">
   <si>
     <t>Additional Info</t>
   </si>
@@ -44,9 +44,6 @@
     <t>[[AP: 5 ]]</t>
   </si>
   <si>
-    <t>[[Range: 3-4 ]]</t>
-  </si>
-  <si>
     <t>[[Modifiable range: Yes ]]</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>[[Area of effect: - Stright line to the end of the map]]</t>
   </si>
   <si>
-    <t>[[Range: 2-00 ]]</t>
-  </si>
-  <si>
     <t>Ignition Arrow</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
     <t>[[Number of turns between two casts: 3 ]]</t>
   </si>
   <si>
-    <t>Burning Ground: [[Area of effect: - 3x3 cells around impact ]]</t>
-  </si>
-  <si>
     <t>Impact: [[Area of effect: - Single cell ]]</t>
   </si>
   <si>
@@ -131,9 +122,6 @@
     <t>Cursed Arrow</t>
   </si>
   <si>
-    <t>[[AP: 7 ]]</t>
-  </si>
-  <si>
     <t>[[Range: 2-3 ]]</t>
   </si>
   <si>
@@ -155,9 +143,6 @@
     <t>Survival</t>
   </si>
   <si>
-    <t>[[AP: 6 ]]</t>
-  </si>
-  <si>
     <t>[[Range: 0 ]]</t>
   </si>
   <si>
@@ -191,48 +176,27 @@
     <t>Canis Lupus skill</t>
   </si>
   <si>
-    <t>On Distortion Area: [[Area of effect: - 3 Singles cells]]</t>
-  </si>
-  <si>
-    <t>Summons a Distortion Area that dosn't block the field of view.  Affect other skills of the caster.</t>
-  </si>
-  <si>
-    <t>Inflicts Light-type damage on enemies.                                        Reduce range of enemies.                                                                                 When targeting the Distortion Area, the skill is replicated on each straight and diagonal line of the Distortion Area and heal caster and allies when touching them.                                                               The first obstacle encountered stop the skill progression.</t>
-  </si>
-  <si>
     <t>Inflicts Light-type damage on impact and Fire-type damage on the burning area.                                                                                     The burning area dealt damage for every burning cell crossed.</t>
   </si>
   <si>
     <t>Increases the caster HP and MP temporarily.                                  Can only be used when the caster has 25% or less HP remaning.</t>
   </si>
   <si>
-    <t>Heal the caster but unsummon the Canis Lupus and preven from summoning it for the rest of the fight.                                              Can only be used when targeting the caster Canis Lupus.</t>
-  </si>
-  <si>
-    <t>Inflicts Wind-type damage on enemies.                                             Push the target.                                                                              When targeting the Distortion Area, the skill is replicated on each straight line of the Distortion Area exept the line of the caster.     The first obstacle encountered stop the skill progression.</t>
-  </si>
-  <si>
-    <t>[[Damage:  25-30 wind ]]</t>
-  </si>
-  <si>
-    <t>Push 2 cells in the opposite direction of the caster.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    [[Damage:  15-20 light ]]</t>
-  </si>
-  <si>
-    <t>If direct hit:</t>
-  </si>
-  <si>
-    <t>If hit from ''Distortion Area'':</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Caster and allies: [[Heal:  15-20 light ]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Ennemies: [[Damage:  15-20 light ]]</t>
-  </si>
-  <si>
+    <t>Inflicts Ground-type damage.                                                         Infinite range and cross every obstacle, but the damage decrease for each obstacle crossed.</t>
+  </si>
+  <si>
+    <t>[[Damage:  (50 - (10 * obstacle crossed)) ground ]]</t>
+  </si>
+  <si>
+    <t>Inflicts Fire-type damage if the caster dosn't have Blood Mark effect, otherwise inflicts Fire-type and Dark-type damage.                                             If the caster dosn't have Blood Mark effect, reduce caster HP and give the effect, otherwise only remove the effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage: 75 fire + 75 dark ]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If caster have </t>
+    </r>
     <r>
       <rPr>
         <sz val="12"/>
@@ -240,7 +204,7 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">    [[Blindness]]</t>
+      <t>[[Blood Mark]]</t>
     </r>
     <r>
       <rPr>
@@ -249,12 +213,299 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> +2 level (2 turns)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    Ennemies: </t>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If caster doesn’t have </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Blood Mark]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage: 75 fire ]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Self: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Blood Mark]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    Self: Remove </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Blood Mark]]</t>
+    </r>
+  </si>
+  <si>
+    <t>Poisons that inflicts Dark-type damage.                                           The poison last longer if the caster have Blood Mark effect.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    [[Poison]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +25 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">    [[Poison]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +25 levels (3 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Vitality]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +15 levels (3 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Speed]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +(Current MP) levels (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>Summon a ''Canis Lupus'' [[25% of caster Max HP, 5 AP, 5 MP, 30% ground resistence, -10% fire resistence, -30% water resistence, 10% wind resistence, -30% light resistence, 30% dark resistence]]</t>
+  </si>
+  <si>
+    <t>Summons a Canis Lupus which poison the enemies.                      Can only be used if the caster is not under the Loneliness effect.</t>
+  </si>
+  <si>
+    <t>Inflicts Ground-type damage and give poisons that inflicts Dark-type damage.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[[Damage: 5-10 ground ]]                                                      </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">[[Poison]] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>+20 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Self: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Loneliness]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>Unsummon ''Canis Lupus''.</t>
+  </si>
+  <si>
+    <t>'Burning Ground'' (Active Glyph) (3 turns):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage: 25 fire ]]</t>
+  </si>
+  <si>
+    <t>Push by 2 cells.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summons a Distortion Area that dosn't block the cell and the field of view. </t>
+  </si>
+  <si>
+    <t>On each line around it every of his starting turn at max 4 ranges:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage: 25 wind]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Push by 2 cells </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inflicts Wind-type damage on enemies.                                             Push the target.                                                                              </t>
+  </si>
+  <si>
+    <t>On enemy: [[Damage:  30-35 wind ]]</t>
+  </si>
+  <si>
+    <t>[[Range: 0-2 ]]</t>
+  </si>
+  <si>
+    <t>Allie: [[Heal: 15-20 light ]]</t>
+  </si>
+  <si>
+    <t>Ennemies: [[Damage:  15-20 light ]]</t>
+  </si>
+  <si>
+    <t>Inflicts Light-type damage on enemies.                                        Reduce range of enemies.                                                                                 Heal allies.</t>
+  </si>
+  <si>
+    <t>[[Range: 00 ]]</t>
+  </si>
+  <si>
+    <t>Burning Ground: [[Area of effect: - cross of 2 cells deep ]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Self: [[Damage: 25% actual HP ]]</t>
+  </si>
+  <si>
+    <t>Heal the caster but unsummon the Canis Lupus and preven from summoning for the rest of the fight.                                                  Can only be used when targeting the caster Canis Lupus.</t>
+  </si>
+  <si>
+    <t>[[AP: 2 ]]</t>
+  </si>
+  <si>
+    <t>[[MP: 2 ]]</t>
+  </si>
+  <si>
+    <t>Self: [[Heal: 25% of Max HP ]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Allie: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Vison]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +2 levels (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ennemies: </t>
     </r>
     <r>
       <rPr>
@@ -272,265 +523,14 @@
         <rFont val="Arial Black"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> +1 level (2 turns)</t>
-    </r>
-  </si>
-  <si>
-    <t>Inflicts Ground-type damage.                                                         Infinite range and cross every obstacle, but the damage decrease for each obstacle crossed.</t>
-  </si>
-  <si>
-    <t>[[Damage:  (50 - (10 * obstacle crossed)) ground ]]</t>
-  </si>
-  <si>
-    <t>Inflicts Fire-type damage if the caster dosn't have Blood Mark effect, otherwise inflicts Fire-type and Dark-type damage.                                             If the caster dosn't have Blood Mark effect, reduce caster HP and give the effect, otherwise only remove the effect.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    [[Damage: 75 fire + 75 dark ]]</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If caster have </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Blood Mark]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If caster doesn’t have </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Blood Mark]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>:</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">    [[Damage: 75 fire ]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Self: [[Damage: 30% Max HP ]]</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    Self: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Blood Mark]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (00 turns)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    Self: Remove </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Blood Mark]]</t>
-    </r>
-  </si>
-  <si>
-    <t>Poisons that inflicts Dark-type damage.                                           The poison last longer if the caster have Blood Mark effect.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    [[Poison]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> +25 levels (2 turns)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">    [[Poison]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> +25 levels (3 turns)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Vitality]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> +15 levels (3 turns)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Speed]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> +(Current MP) levels (1 turn)</t>
-    </r>
-  </si>
-  <si>
-    <t>Summon a ''Canis Lupus'' [[25% of caster Max HP, 5 AP, 5 MP, 30% ground resistence, -10% fire resistence, -30% water resistence, 10% wind resistence, -30% light resistence, 30% dark resistence]]</t>
-  </si>
-  <si>
-    <t>Summons a Canis Lupus which poison the enemies.                      Can only be used if the caster is not under the Loneliness effect.</t>
-  </si>
-  <si>
-    <t>Inflicts Ground-type damage and give poisons that inflicts Dark-type damage.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[[Damage: 5-10 ground ]]                                                      </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">[[Poison]] </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>+20 levels (2 turns)</t>
-    </r>
-  </si>
-  <si>
-    <t>Self: [[Heal: 25% HP ]]</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Self: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t>[[Loneliness]]</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial Black"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (00 turns)</t>
-    </r>
-  </si>
-  <si>
-    <t>Unsummon ''Canis Lupus''.</t>
-  </si>
-  <si>
-    <t>'Burning Ground'' (Active Glyph) (3 turns):</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    [[Damage: 25 fire ]]</t>
+      <t xml:space="preserve"> +2 levels (1 turn)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1028,14 +1028,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1064,7 +1064,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1083,7 +1083,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1095,21 +1095,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1121,7 +1121,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1133,54 +1133,75 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
-        <v>9</v>
+      <c r="C18" s="18" t="s">
+        <v>8</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="19" t="s">
+        <v>73</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B20" s="1"/>
+      <c r="C20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B25" s="1"/>
+      <c r="C25" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="5"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B27" s="1"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1189,14 +1210,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B2:D26"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1213,7 +1234,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1225,7 +1246,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1237,21 +1258,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1263,7 +1284,7 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -1275,7 +1296,7 @@
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1287,7 +1308,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1299,21 +1320,21 @@
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="17" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1357,14 +1378,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1381,7 +1402,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1390,10 +1411,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="15" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1405,14 +1426,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1424,21 +1445,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1450,7 +1471,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1462,68 +1483,61 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="C18" s="18" t="s">
+        <v>77</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="18" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
-      <c r="C20" s="18" t="s">
-        <v>60</v>
-      </c>
+      <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="5"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1532,14 +1546,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B2:D29"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1556,7 +1570,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1565,10 +1579,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="117" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1580,14 +1594,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1599,21 +1613,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1625,7 +1639,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1637,14 +1651,14 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1656,84 +1670,63 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="19" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="19" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="17" t="s">
-        <v>66</v>
+      <c r="C21" s="18" t="s">
+        <v>79</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="19" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
-      <c r="C23" s="19" t="s">
-        <v>64</v>
-      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B24" s="1"/>
-      <c r="C24" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
-      <c r="C25" s="19" t="s">
-        <v>67</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="C26" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="9"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
-      <c r="C29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="5"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1742,14 +1735,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1766,7 +1759,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1778,7 +1771,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1797,7 +1790,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1809,21 +1802,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1835,7 +1828,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1847,7 +1840,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1859,7 +1852,7 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1903,14 +1896,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -1927,7 +1920,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1939,7 +1932,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1958,7 +1951,7 @@
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1970,21 +1963,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1996,7 +1989,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2008,14 +2001,14 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>28</v>
+        <v>83</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2027,21 +2020,21 @@
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="21" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="20" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -2085,14 +2078,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -2109,7 +2102,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2121,7 +2114,7 @@
     <row r="5" spans="2:4" ht="78" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2133,14 +2126,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2152,21 +2145,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2178,7 +2171,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2190,7 +2183,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -2202,49 +2195,49 @@
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
       <c r="C18" s="2" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B23" s="1"/>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
       <c r="C24" s="2" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -2288,14 +2281,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:D29"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -2312,7 +2305,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2324,7 +2317,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2336,14 +2329,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2355,21 +2348,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2381,14 +2374,14 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -2400,7 +2393,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2412,28 +2405,28 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -2477,14 +2470,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B2:D24"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -2501,7 +2494,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2513,7 +2506,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="15" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2525,14 +2518,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2544,7 +2537,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -2556,7 +2549,7 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2568,7 +2561,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2580,14 +2573,14 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="16" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="17" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -2631,14 +2624,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:H26"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="85.7109375" customWidth="1"/>
@@ -2652,7 +2645,7 @@
     <row r="1" spans="2:8" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
       <c r="G1" s="10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2667,12 +2660,12 @@
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2687,12 +2680,12 @@
     <row r="5" spans="2:8" ht="39" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="14" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="14" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2707,19 +2700,19 @@
     <row r="7" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
@@ -2729,12 +2722,12 @@
     <row r="9" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -2749,19 +2742,19 @@
     <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
@@ -2771,7 +2764,7 @@
     <row r="13" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1"/>
       <c r="F13" s="1"/>
@@ -2789,7 +2782,7 @@
     <row r="15" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
@@ -2807,12 +2800,12 @@
     <row r="17" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -2827,12 +2820,12 @@
     <row r="19" spans="2:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="11" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="12" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="H19" s="1"/>
     </row>

</xml_diff>